<commit_message>
Update Selected GPP&TPS for QCC.xlsx
</commit_message>
<xml_diff>
--- a/CD-valid/input/Selected GPP&TPS for QCC.xlsx
+++ b/CD-valid/input/Selected GPP&TPS for QCC.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject-my.sharepoint.com/personal/hortiz_worldjusticeproject_org/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/eu-data-validation/CD-valid/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="8_{792284EC-C976-4462-AD8F-4E5ADC003CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67D1B2F4-9212-4CE2-B7C8-0C920213110E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5606107-9753-854E-AD9A-CCB4D1DA666B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE51C870-9072-4E83-9A26-C2E0A2ABF5A5}"/>
+    <workbookView minimized="1" xWindow="4180" yWindow="2100" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{CE51C870-9072-4E83-9A26-C2E0A2ABF5A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
     <sheet name="Selection and matching" sheetId="1" r:id="rId2"/>
+    <sheet name="Experts matches" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="333">
   <si>
     <t>Special Eurobarometer 489</t>
   </si>
@@ -582,13 +583,593 @@
   </si>
   <si>
     <t>Categorized GPP to TPS matches as follows: High (exact or almost exact match), Medium (similar questions measuring the same concept), Low (suboptimal selection for GPP questions with no obvious match among TPS indicators).</t>
+  </si>
+  <si>
+    <t>PAB_freecourts</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Global GPP</t>
+  </si>
+  <si>
+    <t>2023  EU Questionnaire</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TPS_source</t>
+  </si>
+  <si>
+    <t>TPS_description</t>
+  </si>
+  <si>
+    <t>How often did the government attack the judiciary’s integrity in public?</t>
+  </si>
+  <si>
+    <t>VDEM</t>
+  </si>
+  <si>
+    <t>Sub_pillar</t>
+  </si>
+  <si>
+    <t>CAR_q64_G1</t>
+  </si>
+  <si>
+    <t>q52_G1</t>
+  </si>
+  <si>
+    <t>PAB_attackmedia</t>
+  </si>
+  <si>
+    <t>attack or discredit the media and civil society organizations that criticize them.  Do you agree or disagree that the media and civil society organizations that critique certain entities are targeted and discredited?</t>
+  </si>
+  <si>
+    <t>CAR_q64_G2</t>
+  </si>
+  <si>
+    <t>q52_G2</t>
+  </si>
+  <si>
+    <t>Does the government directly or indirectly attempt to censor the print or broadcast
+media?</t>
+  </si>
+  <si>
+    <t>q46c_G1</t>
+  </si>
+  <si>
+    <t>CPA_media_freeop</t>
+  </si>
+  <si>
+    <t>In [COUNTRY], the media (TV, radio, newspapers)  can freely express opinions against government officials, policies and actions without fear of retaliation. Do you agree or disagree that media freedom to criticize government is important?</t>
+  </si>
+  <si>
+    <t>q39b_G1</t>
+  </si>
+  <si>
+    <t>Are individual journalists harassed — i.e., threatened with libel, arrested, imprisoned,
+beaten, or killed — by governmental or powerful nongovernmental actors while engaged in
+legitimate journalistic activities?</t>
+  </si>
+  <si>
+    <t>In practice, in [COUNTRY], local government officials are elected through a clean process. Do you agree or disagree that clean and fair local government elections are important?</t>
+  </si>
+  <si>
+    <t>q39c_G1</t>
+  </si>
+  <si>
+    <t>CPA_cleanelec_local</t>
+  </si>
+  <si>
+    <t>TPS_variable</t>
+  </si>
+  <si>
+    <t>v2jupoatck</t>
+  </si>
+  <si>
+    <t>v2mecenefm</t>
+  </si>
+  <si>
+    <t>v2meharjrn</t>
+  </si>
+  <si>
+    <t>v2xel_frefair</t>
+  </si>
+  <si>
+    <t>To what extent are elections free and fair?</t>
+  </si>
+  <si>
+    <t>CAR_q65_G2</t>
+  </si>
+  <si>
+    <t>prosecute and convict journalists and leaders of civil society organizations that criticize them. Do you agree or disagree that journalists and leaders of civil society organizations who criticize certain entities are prosecuted and convicted?</t>
+  </si>
+  <si>
+    <t>PAB_prosecutejourn</t>
+  </si>
+  <si>
+    <t>q46a_G2</t>
+  </si>
+  <si>
+    <t>q53_G2</t>
+  </si>
+  <si>
+    <t>In [COUNTRY], people can freely join together with others to draw attention to an issue or sign a petition. Do you agree or disagree that workers' freedom to form labor unions and negotiate with employers is important?</t>
+  </si>
+  <si>
+    <t>q39c_G2</t>
+  </si>
+  <si>
+    <t>CPB_freeassoc</t>
+  </si>
+  <si>
+    <t>To what extent do state authorities respect and protect the right of peaceful assembly?</t>
+  </si>
+  <si>
+    <t>v2caassemb</t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>q43_G2</t>
+  </si>
+  <si>
+    <t>Variable is created by merging Group A and Group B variables</t>
+  </si>
+  <si>
+    <t>CTZ_accountability</t>
+  </si>
+  <si>
+    <t>Assume that a high-ranking government official is taking 
+government money for personal benefit. Assume that one of his employees witnesses this conduct, reports it to the relevant 
+authority, and provides sufficient evidence to prove it. Assume 
+that the press obtains the information and publishes the story. 
+Which one of the following outcomes is most likely?</t>
+  </si>
+  <si>
+    <t>v2lginvstp</t>
+  </si>
+  <si>
+    <t>If the executive were engaged in unconstitutional, illegal, or unethical activity, how likely
+is it that a legislative body (perhaps a whole chamber, perhaps a committee, whether aligned
+with government or opposition) would conduct an investigation that would result in a decision
+or report that is unfavorable to the executive?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Officers working in the local government. How many of the following people in [COUNTRY] do you think are involved in corrupt practices? </t>
+  </si>
+  <si>
+    <t>q2c</t>
+  </si>
+  <si>
+    <t>q3c</t>
+  </si>
+  <si>
+    <t>How often do members of the executive (the head of state, the head of government, and
+cabinet ministers), or their agents, steal, embezzle, or misappropriate public funds or other
+state resources for personal or family use?</t>
+  </si>
+  <si>
+    <t>v2exembez</t>
+  </si>
+  <si>
+    <t>COR_govt_local</t>
+  </si>
+  <si>
+    <t>q2a</t>
+  </si>
+  <si>
+    <t>q3a</t>
+  </si>
+  <si>
+    <t>COR_parliament</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Members of Parliament/Congress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. How many of the following people in [COUNTRY] do you think are involved in corrupt practices? </t>
+    </r>
+  </si>
+  <si>
+    <t>v2lgcrrpt</t>
+  </si>
+  <si>
+    <t>Do members of the legislature abuse their position for financial gain?</t>
+  </si>
+  <si>
+    <t>q48g_G2</t>
+  </si>
+  <si>
+    <t>q44j_G2</t>
+  </si>
+  <si>
+    <t>JSE_indjudges</t>
+  </si>
+  <si>
+    <t>Judges in [COUNTRY] decide cases in an independent manner and are not subject to any sort of pressure. Do you agree or disagree that judges make independent decisions and are not influenced by external pressures?</t>
+  </si>
+  <si>
+    <t>BTI</t>
+  </si>
+  <si>
+    <t>Q3.2 | Independent judiciary</t>
+  </si>
+  <si>
+    <t>Independent judiciary</t>
+  </si>
+  <si>
+    <t>Is there an independent judiciary?</t>
+  </si>
+  <si>
+    <t>Freedom House</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>DIS_religion</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Religion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Such as having or not a religion or religious beliefs?)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Do you feel that you personally experienced any form of discrimination or harassment during the past 12 months</t>
+    </r>
+  </si>
+  <si>
+    <t>EU_q13h</t>
+  </si>
+  <si>
+    <t>q13h</t>
+  </si>
+  <si>
+    <t>Are individuals free to practice and express their religious faith or nonbelief in public and private?</t>
+  </si>
+  <si>
+    <t>DIS_politics</t>
+  </si>
+  <si>
+    <t>EU_q13k</t>
+  </si>
+  <si>
+    <t>q13k</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Political opinion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Such as expressing political views, defending the rights of others, being a member or not of a political party or trade union?)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Do you feel that you personally experienced any form of discrimination or harassment during the past 12 months</t>
+    </r>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>In [COUNTRY], people can freely attend community meetings. Do you agree or disagree that the freedom to attend community meetings is important?</t>
+  </si>
+  <si>
+    <t>CPB_community</t>
+  </si>
+  <si>
+    <t>q46d_G2</t>
+  </si>
+  <si>
+    <t>q39f_G2</t>
+  </si>
+  <si>
+    <t>Is there freedom of assembly?</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>"seek to limit the courts’ competences and freedom to interpret  the law. Do you agree or disagree that seeking to limit the courts' authority and interpretative freedom is a concerning practice?"</t>
+  </si>
+  <si>
+    <t>EU_q4d</t>
+  </si>
+  <si>
+    <t>q4d</t>
+  </si>
+  <si>
+    <t>ORC_govtefforts</t>
+  </si>
+  <si>
+    <t>[NATIONALITY] government efforts to combat corruption are effective. Do you agree or disagree that the government's anti-corruption efforts are successful?</t>
+  </si>
+  <si>
+    <t>Are safeguards against official corruption strong and effective?</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>CJP_proofburden</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Treats those accused of crime as ‘innocent until proven guilty.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Please tell us how confident you are that the criminal justice system as a whole: </t>
+    </r>
+  </si>
+  <si>
+    <t>q49e_G2</t>
+  </si>
+  <si>
+    <t>q44j_G1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Judical Effectiveness</t>
+  </si>
+  <si>
+    <t>Heritage Foundation</t>
+  </si>
+  <si>
+    <t>Properly functioning legal frameworks are essential for protecting the rights of all citizens against unlawful acts by others, including governments and powerful private parties. Judicial e!ectiveness requires effcient and fair judicial systems to ensure that laws are fully respected and appropriate legal actions are taken against violations.</t>
+  </si>
+  <si>
+    <t>CJP_efficient</t>
+  </si>
+  <si>
+    <t>q49b_G1</t>
+  </si>
+  <si>
+    <t>q44b_G1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Deals with cases promptly and efficiently.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Please tell us how confident you are that the criminal justice system as a whole:</t>
+    </r>
+  </si>
+  <si>
+    <t>TRT_police</t>
+  </si>
+  <si>
+    <t>q1d</t>
+  </si>
+  <si>
+    <t>q1e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The police. Please tell me, how much TRUST do you have in each of the following categories of people, groups of people, and institutions? </t>
+  </si>
+  <si>
+    <t>Economic Freedom in the World</t>
+  </si>
+  <si>
+    <t>2H Reliability of police</t>
+  </si>
+  <si>
+    <t>Reliability of police</t>
+  </si>
+  <si>
+    <t>Do laws, policies, and practices guarantee equal treatment of various segments of the population?</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>ROL_equality_sig</t>
+  </si>
+  <si>
+    <t>ROL_equality_imp</t>
+  </si>
+  <si>
+    <t>The same laws and rules apply equally to every person, including all public authorities, irrespective of their personal circumstances, social status, wealth, political connections or origin</t>
+  </si>
+  <si>
+    <t>EU_q58a</t>
+  </si>
+  <si>
+    <t>q58a</t>
+  </si>
+  <si>
+    <t>EU_q59a</t>
+  </si>
+  <si>
+    <t>q59a</t>
+  </si>
+  <si>
+    <t>Sub_pillar_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pillar_2 </t>
+  </si>
+  <si>
+    <t>Pillar_3</t>
+  </si>
+  <si>
+    <t>Sub_pillar_3</t>
+  </si>
+  <si>
+    <t>v2x_jucon</t>
+  </si>
+  <si>
+    <t>To what extent does the executive respect the constitution and comply with court
+rulings, and to what extent is the judiciary able to act in an independent fashion?</t>
+  </si>
+  <si>
+    <t>JSE_polinfluence</t>
+  </si>
+  <si>
+    <t>EU_q44i_G2</t>
+  </si>
+  <si>
+    <t>q44i_G2</t>
+  </si>
+  <si>
+    <t>Local courts are free of political influence in their application of power. Do you agree or disagree that local courts are not subject to political influence in their actions?</t>
+  </si>
+  <si>
+    <t>To what extent are parties, including opposition parties, allowed to form and to
+participate in elections, and to what extent are civil society organizations able to form and to operate freely?</t>
+  </si>
+  <si>
+    <t>v2x_frassoc_thick</t>
+  </si>
+  <si>
+    <t>prosecute and convict members of opposition parties. Do you agree or disagree that prosecuting and convicting members of opposition parties is a concerning practice?</t>
+  </si>
+  <si>
+    <t>CAR_q68_G1</t>
+  </si>
+  <si>
+    <t>q56_G1</t>
+  </si>
+  <si>
+    <t>PAB_prosecuteopp</t>
+  </si>
+  <si>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>1.04</t>
+  </si>
+  <si>
+    <t>2.03</t>
+  </si>
+  <si>
+    <t>2.01</t>
+  </si>
+  <si>
+    <t>1.02</t>
+  </si>
+  <si>
+    <t>4.03</t>
+  </si>
+  <si>
+    <t>4.02</t>
+  </si>
+  <si>
+    <t>4.06</t>
+  </si>
+  <si>
+    <t>8.01</t>
+  </si>
+  <si>
+    <t>3.02</t>
+  </si>
+  <si>
+    <t>7.04</t>
+  </si>
+  <si>
+    <t>8.06</t>
+  </si>
+  <si>
+    <t>Taking all aspects of the pre-election period, election day, and the post-election process
+into account, would you consider subnational elections (regional and local, as previously
+identified) to be free and fair on average?</t>
+  </si>
+  <si>
+    <t>v2elffelr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,8 +1232,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -707,6 +1313,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -755,10 +1367,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -774,39 +1387,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -817,11 +1416,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D4CF4182-91B5-9D44-A423-3CCA9918B0A9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -837,7 +1461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1139,202 +1763,202 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="34" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="25">
         <v>72</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="24" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="34" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="25">
         <v>58</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="25">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="25">
         <v>56</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="25">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="36" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="37">
-        <v>13</v>
-      </c>
-      <c r="E10" s="35" t="s">
+      <c r="C10" s="27">
+        <v>13</v>
+      </c>
+      <c r="E10" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="25">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="36"/>
-      <c r="C11" s="37" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="F11" s="35">
+      <c r="F11" s="25">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
-      <c r="C12" s="41" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="30"/>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="25">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="40"/>
-      <c r="C13" s="41" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="30"/>
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="40"/>
-      <c r="C14" s="41" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="30"/>
+      <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="25">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
-      <c r="C15" s="41" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="30"/>
+      <c r="C15" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="25">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="40"/>
-      <c r="C16" s="41" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="30"/>
+      <c r="C16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="40"/>
-      <c r="C17" s="41" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="30"/>
+      <c r="C17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="30"/>
+      <c r="C18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="40"/>
-      <c r="C19" s="41" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="30"/>
+      <c r="C19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="40"/>
-      <c r="C20" s="41" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="30"/>
+      <c r="C20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="30"/>
+      <c r="C21" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="30"/>
+      <c r="C22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="38"/>
-      <c r="C23" s="39" t="s">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="38" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="39">
+      <c r="C24" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1348,61 +1972,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7F1BD1-5518-4A5D-9F8E-120B4A3F3ED6}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="43.33203125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" style="9" customWidth="1"/>
-    <col min="6" max="8" width="11.5546875" style="9"/>
+    <col min="2" max="4" width="43.36328125" customWidth="1"/>
+    <col min="5" max="5" width="26.6328125" customWidth="1"/>
+    <col min="6" max="8" width="11.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="26">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="18">
         <v>1.01</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="27" t="s">
+      <c r="B2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="str">
@@ -1410,26 +2034,26 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1.02</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3">
         <v>2019</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" t="s">
         <v>52</v>
       </c>
       <c r="I3" t="str">
@@ -1437,26 +2061,26 @@
         <v xml:space="preserve">Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:Judges in [COUNTRY] decide cases in an independent manner and are not subject to any sort of pressure. </v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1.02</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4">
         <v>2019</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" t="s">
         <v>52</v>
       </c>
       <c r="I4" t="str">
@@ -1464,26 +2088,26 @@
         <v>Please tell me whether the following points need to be improved in OUR COUNTRY:(f) Public authorities and politicians respect and apply court rulings</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1.03</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5">
         <v>2023</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" t="s">
         <v>52</v>
       </c>
       <c r="I5" t="str">
@@ -1491,26 +2115,26 @@
         <v>Please tell me whether you agree or disagree with each of the following?(NATIONALITY) Government efforts to combat corruption are effective</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1.03</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6">
         <v>2023</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="I6" t="str">
@@ -1518,26 +2142,26 @@
         <v>Please tell me whether you agree or disagree with each of the following?In (OUR COUNTRY), measures against corruption are applied impartially and without ulterior motives</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1.04</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7">
         <v>2021</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" t="s">
         <v>50</v>
       </c>
       <c r="I7" t="str">
@@ -1545,26 +2169,26 @@
         <v>In practice, in [COUNTRY], people can vote freely without feeling harassed or pressuredNA</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1.04</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8">
         <v>2023</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" t="s">
         <v>55</v>
       </c>
       <c r="I8" t="str">
@@ -1572,26 +2196,26 @@
         <v>In practice, in [COUNTRY], local government officials are elected through a clean processNA</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1.05</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
         <v>2019</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" t="s">
         <v>52</v>
       </c>
       <c r="I9" t="str">
@@ -1599,26 +2223,26 @@
         <v>In [COUNTRY], the media (TV, radio, newspapers)  can freely express opinions against government officials, policies and actions without fear of retaliationNA</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1.05</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10">
         <v>2019</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" t="s">
         <v>52</v>
       </c>
       <c r="I10" t="str">
@@ -1626,14 +2250,14 @@
         <v>In [COUNTRY], civil society organizations can freely express opinions against government policies and actions without fear of retaliationNA</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1.05</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="s">
@@ -1642,10 +2266,10 @@
       <c r="E11" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11">
         <v>2023</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" t="s">
         <v>50</v>
       </c>
       <c r="I11" t="str">
@@ -1653,14 +2277,14 @@
         <v>In practice, in [COUNTRY], people can freely join any (unforbidden) political organization they wantNA</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1.05</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
@@ -1669,10 +2293,10 @@
       <c r="E12" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12">
         <v>2023</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" t="s">
         <v>50</v>
       </c>
       <c r="I12" t="str">
@@ -1680,26 +2304,26 @@
         <v>In [COUNTRY], people can freely express opinions against the governmentNA</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1.06</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13">
         <v>2023</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" t="s">
         <v>55</v>
       </c>
       <c r="I13" t="str">
@@ -1707,26 +2331,26 @@
         <v xml:space="preserve">In [COUNTRY], top government officials of the national government …… use emergency powers to bypass institutional checks and balances. </v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1.07</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14">
         <v>2023</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" t="s">
         <v>50</v>
       </c>
       <c r="I14" t="str">
@@ -1734,26 +2358,26 @@
         <v xml:space="preserve">In [COUNTRY], top government officials of the national government …… refuse to comply with court rulings that are not in their favor. </v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1.08</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
         <v>13</v>
       </c>
       <c r="I15" t="str">
@@ -1761,26 +2385,26 @@
         <v xml:space="preserve">Please tell me whether the following points need to be improved in OUR COUNTRY:(h) Public authorities respect the competences, mandates, and legal powers of independent government bodies or other autonomous authorities.  </v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1.0900000000000001</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16">
         <v>2021</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" t="s">
         <v>52</v>
       </c>
       <c r="I16" t="str">
@@ -1788,26 +2412,26 @@
         <v xml:space="preserve">In [COUNTRY], top government officials of the national government …… manipulate the election process to win power. </v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17">
         <v>2023</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" t="s">
         <v>50</v>
       </c>
       <c r="I17" t="str">
@@ -1815,26 +2439,26 @@
         <v xml:space="preserve">In [COUNTRY], top government officials of the national government …… attack or discredit the media and civil society organizations that criticize them. </v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18">
         <v>2021</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" t="s">
         <v>55</v>
       </c>
       <c r="I18" t="str">
@@ -1842,26 +2466,26 @@
         <v>In [COUNTRY], top government officials of the national government …… use misinformation to shape public opinion in their favor.</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1.1100000000000001</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19">
         <v>2019</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" t="s">
         <v>52</v>
       </c>
       <c r="I19" t="str">
@@ -1869,26 +2493,26 @@
         <v>Please tell me whether the following points need to be improved in OUR COUNTRY:(d) Corruption involving public officials and politicians is properly investigated and those responsible are brought to justice</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>2021</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" t="s">
         <v>50</v>
       </c>
       <c r="I20" t="str">
@@ -1896,26 +2520,26 @@
         <v>In talking to people about their local government, we often find important differences in how well the government, police, and the courts perform their jobs. Please tell me to what extent do you agree that:In [COUNTRY], if members of the police request bribes from the public, they will be held accountable</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>2.1</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2023</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" t="s">
         <v>52</v>
       </c>
       <c r="I21" t="str">
@@ -1923,26 +2547,26 @@
         <v>Please tell me whether you agree or disagree with each of the following?You are personally affected by corruption in your daily life</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>2.1</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="C22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22">
         <v>2023</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" t="s">
         <v>52</v>
       </c>
       <c r="I22" t="str">
@@ -1950,26 +2574,26 @@
         <v>In the past three years, would you say that the level of corruption in (OUR COUNTRY) has…? NA</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>2.1</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>2023</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" t="s">
         <v>52</v>
       </c>
       <c r="I23" t="str">
@@ -1977,26 +2601,26 @@
         <v>In the last three years, did you use any PUBLIC health services?Did you have to pay a bribe to receive the service or expedite the process?</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>2.1</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>2021</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G24" t="s">
         <v>50</v>
       </c>
       <c r="I24" t="str">
@@ -2004,26 +2628,26 @@
         <v>In the last three years, did you request a government permit, or process any kind of document (like a license, building permit, etc.) in a local government office?Did you have to pay a bribe to receive the service or expedite the process?</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="26">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B25" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="27" t="s">
+      <c r="B25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I25" t="str">
@@ -2031,26 +2655,26 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="27" t="s">
+      <c r="B26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I26" t="str">
@@ -2058,26 +2682,26 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>2.4</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" t="s">
         <v>0</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>2019</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" t="s">
         <v>52</v>
       </c>
       <c r="I27" t="str">
@@ -2085,26 +2709,26 @@
         <v>Please tell me whether the following points need to be improved in OUR COUNTRY:(c) Public officials and politicians do not use their positions to obtain benefits for themselves or their family members but take decisions in the public interest</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>2.4</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>2023</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" t="s">
         <v>52</v>
       </c>
       <c r="I28" t="str">
@@ -2112,26 +2736,26 @@
         <v>Please tell me whether you agree or disagree with each of the following?In (OUR COUNTRY) the only way to succeed in business is to have political connections</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="26">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="18">
         <v>2.5</v>
       </c>
-      <c r="B29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="27" t="s">
+      <c r="B29" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I29" t="str">
@@ -2139,14 +2763,14 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>3.1</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="14" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2155,10 +2779,10 @@
       <c r="E30" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30">
         <v>2023</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" t="s">
         <v>50</v>
       </c>
       <c r="I30" t="str">
@@ -2166,14 +2790,14 @@
         <v>If you were to request to have access to these documents, how likely do you think it is that the government agency will grant it, assuming the information is properly requested? Would you say that it is very likely, likely, unlikely, or very unlikely?Sources of campaign financing of elected officials and legislators</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>3.1</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="15" t="s">
         <v>49</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2182,10 +2806,10 @@
       <c r="E31" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31">
         <v>2019</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" t="s">
         <v>52</v>
       </c>
       <c r="I31" t="str">
@@ -2193,14 +2817,14 @@
         <v>To what extent do you agree or disagree with each of the following statements. Local authorities: Provide information for people in a simple, easy-to-read way</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>3.1</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2209,10 +2833,10 @@
       <c r="E32" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32">
         <v>2019</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" t="s">
         <v>52</v>
       </c>
       <c r="I32" t="str">
@@ -2220,14 +2844,14 @@
         <v>To what extent do you agree or disagree with each of the following statements. Local authorities: Provide people with information about their rights</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>3.1</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="15" t="s">
         <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2236,10 +2860,10 @@
       <c r="E33" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33">
         <v>2019</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" t="s">
         <v>52</v>
       </c>
       <c r="I33" t="str">
@@ -2247,14 +2871,14 @@
         <v>To what extent do you agree or disagree with each of the following statements. Local authorities: Make information easy to find online</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>3.1</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="15" t="s">
         <v>79</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2263,10 +2887,10 @@
       <c r="E34" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34">
         <v>2019</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G34" t="s">
         <v>52</v>
       </c>
       <c r="I34" t="str">
@@ -2274,26 +2898,26 @@
         <v>To what extent do you agree or disagree with each of the following statements. Local authorities: Make information easy to find without using the internet, such as using leaflets or posters</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>3.2</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="14" t="s">
+      <c r="C35" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" t="s">
         <v>0</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35">
         <v>2019</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G35" t="s">
         <v>52</v>
       </c>
       <c r="I35" t="str">
@@ -2301,26 +2925,26 @@
         <v>In [COUNTRY], the media (TV, radio, newspapers)  can freely express opinions against government officials, policies and actions without fear of retaliationNA</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="6">
         <v>3.2</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="14" t="s">
+      <c r="C36" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" t="s">
         <v>0</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F36">
         <v>2019</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" t="s">
         <v>52</v>
       </c>
       <c r="I36" t="str">
@@ -2328,14 +2952,14 @@
         <v>In [COUNTRY], civil society organizations can freely express opinions against government policies and actions without fear of retaliationNA</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="6">
         <v>3.2</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D37" t="s">
@@ -2344,10 +2968,10 @@
       <c r="E37" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37">
         <v>2023</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" t="s">
         <v>50</v>
       </c>
       <c r="I37" t="str">
@@ -2355,14 +2979,14 @@
         <v>In practice, in [COUNTRY], people can freely join any (unforbidden) political organization they wantNA</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="6">
         <v>3.2</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D38" t="s">
@@ -2371,10 +2995,10 @@
       <c r="E38" t="s">
         <v>89</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38">
         <v>2023</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" t="s">
         <v>50</v>
       </c>
       <c r="I38" t="str">
@@ -2382,14 +3006,14 @@
         <v>In [COUNTRY], people can freely express opinions against the governmentNA</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="6">
         <v>3.2</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="12" t="s">
         <v>86</v>
       </c>
       <c r="D39" t="s">
@@ -2398,10 +3022,10 @@
       <c r="E39" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="9">
+      <c r="F39">
         <v>2020</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" t="s">
         <v>52</v>
       </c>
       <c r="I39" t="str">
@@ -2409,14 +3033,14 @@
         <v>There are different ways of trying to improve things in [COUNTRY] or help prevent things from going wrong. During the past 12 months, have you:Attended a legal demonstration or protest march?</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="6">
         <v>3.2</v>
       </c>
       <c r="B40" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="12" t="s">
         <v>87</v>
       </c>
       <c r="D40" t="s">
@@ -2425,10 +3049,10 @@
       <c r="E40" t="s">
         <v>83</v>
       </c>
-      <c r="F40" s="9">
+      <c r="F40">
         <v>2020</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G40" t="s">
         <v>52</v>
       </c>
       <c r="I40" t="str">
@@ -2438,7 +3062,7 @@
 money?</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="6">
         <v>3.2</v>
       </c>
@@ -2454,10 +3078,10 @@
       <c r="E41" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41">
         <v>2020</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" t="s">
         <v>52</v>
       </c>
       <c r="I41" t="str">
@@ -2465,7 +3089,7 @@
         <v>Please tell me, how much TRUST do you have in each of the following categories of people, groups of people, and institutions?Members of Parliament/Congress</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="6">
         <v>3.2</v>
       </c>
@@ -2481,10 +3105,10 @@
       <c r="E42" t="s">
         <v>83</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42">
         <v>2020</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G42" t="s">
         <v>52</v>
       </c>
       <c r="I42" t="str">
@@ -2492,7 +3116,7 @@
         <v>Please tell me, how much TRUST do you have in each of the following categories of people, groups of people, and institutions?The police</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="6">
         <v>3.2</v>
       </c>
@@ -2508,10 +3132,10 @@
       <c r="E43" t="s">
         <v>83</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43">
         <v>2020</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" t="s">
         <v>52</v>
       </c>
       <c r="I43" t="str">
@@ -2519,26 +3143,26 @@
         <v>Please tell me, how much TRUST do you have in each of the following categories of people, groups of people, and institutions?Political parties</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="26">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B44" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="27" t="s">
+      <c r="B44" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I44" t="str">
@@ -2546,26 +3170,26 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="30">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="20">
         <v>4.2</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="14" t="s">
+      <c r="C45" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" t="s">
         <v>0</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45">
         <v>2019</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G45" t="s">
         <v>52</v>
       </c>
       <c r="I45" t="str">
@@ -2573,26 +3197,26 @@
         <v>In [COUNTRY], the media (TV, radio, newspapers)  can freely express opinions against government officials, policies and actions without fear of retaliationNA</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="30">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="20">
         <v>4.2</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C46" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="14" t="s">
+      <c r="C46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" t="s">
         <v>0</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46">
         <v>2019</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G46" t="s">
         <v>52</v>
       </c>
       <c r="I46" t="str">
@@ -2600,14 +3224,14 @@
         <v>In [COUNTRY], civil society organizations can freely express opinions against government policies and actions without fear of retaliationNA</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="30">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="20">
         <v>4.2</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D47" t="s">
@@ -2616,10 +3240,10 @@
       <c r="E47" t="s">
         <v>89</v>
       </c>
-      <c r="F47" s="9">
+      <c r="F47">
         <v>2023</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" t="s">
         <v>50</v>
       </c>
       <c r="I47" t="str">
@@ -2627,14 +3251,14 @@
         <v>In practice, in [COUNTRY], people can freely join any (unforbidden) political organization they wantNA</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="30">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="20">
         <v>4.2</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D48" t="s">
@@ -2643,10 +3267,10 @@
       <c r="E48" t="s">
         <v>89</v>
       </c>
-      <c r="F48" s="9">
+      <c r="F48">
         <v>2023</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G48" t="s">
         <v>50</v>
       </c>
       <c r="I48" t="str">
@@ -2654,8 +3278,8 @@
         <v>In [COUNTRY], people can freely express opinions against the governmentNA</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="30">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="20">
         <v>4.3</v>
       </c>
       <c r="B49" t="s">
@@ -2670,10 +3294,10 @@
       <c r="E49" t="s">
         <v>0</v>
       </c>
-      <c r="F49" s="9">
+      <c r="F49">
         <v>2019</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" t="s">
         <v>52</v>
       </c>
       <c r="I49" t="str">
@@ -2681,8 +3305,8 @@
         <v>Please tell me whether the following points need to be improved in OUR COUNTRY:(a) The same laws and rules apply equally to every person, including all public authorities, irrespective of their personal circumstances, social status, wealth, political connections or origin</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="30">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="20">
         <v>4.4000000000000004</v>
       </c>
       <c r="B50" t="s">
@@ -2697,10 +3321,10 @@
       <c r="E50" t="s">
         <v>104</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50">
         <v>2021</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" t="s">
         <v>50</v>
       </c>
       <c r="I50" t="str">
@@ -2708,8 +3332,8 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements that I am going to read. Based on your experience or on what you have heard, would you say that: In [COUNTRY], working conditions are good, including working time, work organization, health and safety at work, employee representation, and relation with the employer.</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="30">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="20">
         <v>4.4000000000000004</v>
       </c>
       <c r="B51" t="s">
@@ -2724,10 +3348,10 @@
       <c r="E51" t="s">
         <v>104</v>
       </c>
-      <c r="F51" s="9">
+      <c r="F51">
         <v>2021</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" t="s">
         <v>50</v>
       </c>
       <c r="I51" t="str">
@@ -2735,26 +3359,26 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements that I am going to read. Based on your experience or on what you have heard, would you say that: In [COUNTRY], working conditions are good, including working time, work organization, health and safety at work, employee representation, and relation with the employer.</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="30">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="20">
         <v>4.5</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="14" t="s">
+      <c r="C52" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" t="s">
         <v>25</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F52">
         <v>2021</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" t="s">
         <v>50</v>
       </c>
       <c r="I52" t="str">
@@ -2762,14 +3386,14 @@
         <v>In practice, in [COUNTRY], people can vote freely without feeling harassed or pressuredNA</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="30">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="20">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="10" t="s">
         <v>109</v>
       </c>
       <c r="D53" t="s">
@@ -2778,10 +3402,10 @@
       <c r="E53" t="s">
         <v>83</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F53">
         <v>2020</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" t="s">
         <v>52</v>
       </c>
       <c r="I53" t="str">
@@ -2789,8 +3413,8 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:All parties are treated equally and fairly within the civil justice system.</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="30">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="20">
         <v>4.5999999999999996</v>
       </c>
       <c r="B54" t="s">
@@ -2805,10 +3429,10 @@
       <c r="E54" t="s">
         <v>0</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F54">
         <v>2019</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G54" t="s">
         <v>52</v>
       </c>
       <c r="I54" t="str">
@@ -2816,8 +3440,8 @@
         <v>Please tell me whether the following points need to be improved in OUR COUNTRY:(e) If your rights are not respected, you can have them upheld by an independent court</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="30">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="20">
         <v>4.5999999999999996</v>
       </c>
       <c r="B55" s="8" t="s">
@@ -2832,10 +3456,10 @@
       <c r="E55" t="s">
         <v>89</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F55">
         <v>2023</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G55" t="s">
         <v>55</v>
       </c>
       <c r="I55" t="str">
@@ -2843,8 +3467,8 @@
         <v>Please tell us how confident you are that the criminal justice system as a whole:Treats those accused of crime as 'innocent until proven guilty'.</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="31">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="21">
         <v>5.0999999999999996</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -2859,10 +3483,10 @@
       <c r="E56" t="s">
         <v>114</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F56">
         <v>2020</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" t="s">
         <v>52</v>
       </c>
       <c r="I56" t="str">
@@ -2870,8 +3494,8 @@
         <v>How safe do you feel walking in your neighborhood at night?NA</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="31">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="21">
         <v>5.2</v>
       </c>
       <c r="B57" t="s">
@@ -2886,10 +3510,10 @@
       <c r="E57" t="s">
         <v>116</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F57">
         <v>2022</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G57" t="s">
         <v>55</v>
       </c>
       <c r="I57" t="str">
@@ -2897,8 +3521,8 @@
         <v>Do you know or have you heard if the following situations happen or occur around your home?Police violence against people</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="31">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="21">
         <v>5.2</v>
       </c>
       <c r="B58" t="s">
@@ -2913,10 +3537,10 @@
       <c r="E58" t="s">
         <v>116</v>
       </c>
-      <c r="F58" s="9">
+      <c r="F58">
         <v>2022</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="G58" t="s">
         <v>50</v>
       </c>
       <c r="I58" t="str">
@@ -2924,8 +3548,8 @@
         <v>Do you know or have you heard if the following situations happen or occur around your home?Racially motivated violence</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="31">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="21">
         <v>5.2</v>
       </c>
       <c r="B59" t="s">
@@ -2940,10 +3564,10 @@
       <c r="E59" t="s">
         <v>116</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59">
         <v>2022</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="G59" t="s">
         <v>55</v>
       </c>
       <c r="I59" t="str">
@@ -2951,8 +3575,8 @@
         <v>Do you know or have you heard if the following situations happen or occur around your home?Organized crime</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="31">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="21">
         <v>5.2</v>
       </c>
       <c r="B60" t="s">
@@ -2967,10 +3591,10 @@
       <c r="E60" t="s">
         <v>116</v>
       </c>
-      <c r="F60" s="9">
+      <c r="F60">
         <v>2022</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="G60" t="s">
         <v>52</v>
       </c>
       <c r="I60" t="str">
@@ -2978,8 +3602,8 @@
         <v>Do you know or have you heard if the following situations happen or occur around your home?Street violence (violent property crime, violent injury, gun violence)</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="31">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="21">
         <v>5.2</v>
       </c>
       <c r="B61" t="s">
@@ -2994,10 +3618,10 @@
       <c r="E61" t="s">
         <v>116</v>
       </c>
-      <c r="F61" s="9">
+      <c r="F61">
         <v>2022</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="G61" t="s">
         <v>55</v>
       </c>
       <c r="I61" t="str">
@@ -3005,26 +3629,26 @@
         <v>Do you know or have you heard if the following situations happen or occur around your home?Violence against women</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="26">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="18">
         <v>6.1</v>
       </c>
-      <c r="B62" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G62" s="27" t="s">
+      <c r="B62" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I62" t="str">
@@ -3032,26 +3656,26 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="26">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="18">
         <v>6.2</v>
       </c>
-      <c r="B63" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E63" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F63" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G63" s="27" t="s">
+      <c r="B63" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I63" t="str">
@@ -3059,26 +3683,26 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="26">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="18">
         <v>6.3</v>
       </c>
-      <c r="B64" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E64" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="27" t="s">
+      <c r="B64" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I64" t="str">
@@ -3086,14 +3710,14 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="32">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" s="22">
         <v>7.1</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="13" t="s">
+      <c r="C65" s="10" t="s">
         <v>129</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -3102,10 +3726,10 @@
       <c r="E65" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="9">
+      <c r="F65">
         <v>2019</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" t="s">
         <v>55</v>
       </c>
       <c r="I65" t="str">
@@ -3113,14 +3737,14 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:People are aware of their rights when they face a legal problem.</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="32">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="22">
         <v>7.2</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="10" t="s">
         <v>130</v>
       </c>
       <c r="D66" s="4" t="s">
@@ -3129,13 +3753,13 @@
       <c r="E66" t="s">
         <v>40</v>
       </c>
-      <c r="F66" s="9">
+      <c r="F66">
         <v>2023</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" t="s">
         <v>55</v>
       </c>
-      <c r="H66" s="11" t="s">
+      <c r="H66" t="s">
         <v>133</v>
       </c>
       <c r="I66" t="str">
@@ -3143,14 +3767,14 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:People have access to affordable legal assistance and representation when they face a legal problem.</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="32">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="22">
         <v>7.2</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="10" t="s">
         <v>130</v>
       </c>
       <c r="D67" s="4" t="s">
@@ -3159,13 +3783,13 @@
       <c r="E67" t="s">
         <v>40</v>
       </c>
-      <c r="F67" s="9">
+      <c r="F67">
         <v>2023</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="G67" t="s">
         <v>55</v>
       </c>
-      <c r="H67" s="11" t="s">
+      <c r="H67" t="s">
         <v>133</v>
       </c>
       <c r="I67" t="str">
@@ -3173,14 +3797,14 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:People have access to affordable legal assistance and representation when they face a legal problem.</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="32">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="22">
         <v>7.3</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="13" t="s">
+      <c r="C68" s="10" t="s">
         <v>135</v>
       </c>
       <c r="D68" t="s">
@@ -3189,13 +3813,13 @@
       <c r="E68" t="s">
         <v>0</v>
       </c>
-      <c r="F68" s="9">
+      <c r="F68">
         <v>2019</v>
       </c>
-      <c r="G68" s="11" t="s">
+      <c r="G68" t="s">
         <v>52</v>
       </c>
-      <c r="H68" s="11" t="s">
+      <c r="H68" t="s">
         <v>137</v>
       </c>
       <c r="I68" t="str">
@@ -3203,14 +3827,14 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:People can easily meet the costs of turning to a state dispute resolution mechanisms (courts, small claims courts, administrative agencies, etc.) when they face a legal problem.</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="32">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="22">
         <v>7.3</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="10" t="s">
         <v>136</v>
       </c>
       <c r="D69" t="s">
@@ -3219,13 +3843,13 @@
       <c r="E69" t="s">
         <v>0</v>
       </c>
-      <c r="F69" s="9">
+      <c r="F69">
         <v>2019</v>
       </c>
-      <c r="G69" s="11" t="s">
+      <c r="G69" t="s">
         <v>52</v>
       </c>
-      <c r="H69" s="11" t="s">
+      <c r="H69" t="s">
         <v>138</v>
       </c>
       <c r="I69" t="str">
@@ -3233,29 +3857,29 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:Civil and commercial courts adjudicate disputes quickly (starting from the moment the case is filed to the moment a decision or agreement is reached).</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="32">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="22">
         <v>7.4</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C70" s="13" t="s">
+      <c r="C70" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" t="s">
         <v>0</v>
       </c>
-      <c r="F70" s="9">
+      <c r="F70">
         <v>2019</v>
       </c>
-      <c r="G70" s="9" t="s">
+      <c r="G70" t="s">
         <v>52</v>
       </c>
-      <c r="H70" s="9" t="s">
+      <c r="H70" t="s">
         <v>153</v>
       </c>
       <c r="I70" t="str">
@@ -3263,8 +3887,8 @@
         <v xml:space="preserve">Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:Judges in [COUNTRY] decide cases in an independent manner and are not subject to any sort of pressure. </v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="32">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="22">
         <v>7.4</v>
       </c>
       <c r="B71" s="8" t="s">
@@ -3276,16 +3900,16 @@
       <c r="D71" t="s">
         <v>141</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E71" t="s">
         <v>58</v>
       </c>
-      <c r="F71" s="9">
+      <c r="F71">
         <v>2021</v>
       </c>
-      <c r="G71" s="9" t="s">
+      <c r="G71" t="s">
         <v>52</v>
       </c>
-      <c r="H71" s="9" t="s">
+      <c r="H71" t="s">
         <v>153</v>
       </c>
       <c r="I71" t="str">
@@ -3293,14 +3917,14 @@
         <v>How many of the following people in [COUNTRY] do you think are involved in corrupt practices?Judges and Magistrates</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="32">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="22">
         <v>7.5</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="10" t="s">
         <v>142</v>
       </c>
       <c r="D72" t="s">
@@ -3309,10 +3933,10 @@
       <c r="E72" t="s">
         <v>0</v>
       </c>
-      <c r="F72" s="9">
+      <c r="F72">
         <v>2019</v>
       </c>
-      <c r="G72" s="9" t="s">
+      <c r="G72" t="s">
         <v>159</v>
       </c>
       <c r="I72" t="str">
@@ -3320,14 +3944,14 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:Winning parties can enforce court decisions quickly and effectively.</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="32">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="22">
         <v>7.6</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="10" t="s">
         <v>144</v>
       </c>
       <c r="D73" t="s">
@@ -3336,10 +3960,10 @@
       <c r="E73" t="s">
         <v>146</v>
       </c>
-      <c r="F73" s="9">
+      <c r="F73">
         <v>2023</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G73" t="s">
         <v>159</v>
       </c>
       <c r="I73" t="str">
@@ -3347,8 +3971,8 @@
         <v>Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:People can easily turn to alternative justice mechanisms (mediation, arbitration, restorative justice, etc.) when they face a legal problem.</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="33">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="23">
         <v>8.1</v>
       </c>
       <c r="B74" t="s">
@@ -3363,13 +3987,13 @@
       <c r="E74" t="s">
         <v>0</v>
       </c>
-      <c r="F74" s="9">
+      <c r="F74">
         <v>2019</v>
       </c>
-      <c r="G74" s="9" t="s">
+      <c r="G74" t="s">
         <v>52</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="H74" t="s">
         <v>152</v>
       </c>
       <c r="I74" t="str">
@@ -3377,8 +4001,8 @@
         <v xml:space="preserve">In talking to people about their local government, we often find important differences in how well the government, police, and the courts perform their jobs. Please tell me to what extent do you agree that:Police investigators in [COUNTRY] investigate crimes in an independent manner and are not subject to any sort of pressure. </v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="33">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="23">
         <v>8.1</v>
       </c>
       <c r="B75" s="8" t="s">
@@ -3393,10 +4017,10 @@
       <c r="E75" t="s">
         <v>58</v>
       </c>
-      <c r="F75" s="9">
+      <c r="F75">
         <v>2021</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G75" t="s">
         <v>52</v>
       </c>
       <c r="I75" t="str">
@@ -3404,14 +4028,14 @@
         <v>How many of the following people in [COUNTRY] do you think are involved in corrupt practices?Police officers</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="33">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="23">
         <v>8.1999999999999993</v>
       </c>
       <c r="B76" t="s">
         <v>16</v>
       </c>
-      <c r="C76" s="13" t="s">
+      <c r="C76" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D76" t="s">
@@ -3420,13 +4044,13 @@
       <c r="E76" t="s">
         <v>0</v>
       </c>
-      <c r="F76" s="9">
+      <c r="F76">
         <v>2019</v>
       </c>
-      <c r="G76" s="9" t="s">
+      <c r="G76" t="s">
         <v>52</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="H76" t="s">
         <v>152</v>
       </c>
       <c r="I76" t="str">
@@ -3434,8 +4058,8 @@
         <v xml:space="preserve">In talking to people about their local government, we often find important differences in how well the government, police, and the courts perform their jobs. Please tell me to what extent do you agree that:Prosecutors in [COUNTRY] prosecute crimes committed in an independent manner and are not subject to any sort of pressure. </v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="33">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="23">
         <v>8.3000000000000007</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -3447,16 +4071,16 @@
       <c r="D77" t="s">
         <v>141</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" t="s">
         <v>58</v>
       </c>
-      <c r="F77" s="9">
+      <c r="F77">
         <v>2021</v>
       </c>
-      <c r="G77" s="9" t="s">
+      <c r="G77" t="s">
         <v>52</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="H77" t="s">
         <v>154</v>
       </c>
       <c r="I77" t="str">
@@ -3464,29 +4088,29 @@
         <v>How many of the following people in [COUNTRY] do you think are involved in corrupt practices?Judges and Magistrates</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="33">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="23">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B78" s="13" t="s">
+      <c r="B78" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D78" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E78" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="9">
+      <c r="F78">
         <v>2019</v>
       </c>
-      <c r="G78" s="9" t="s">
+      <c r="G78" t="s">
         <v>52</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="H78" t="s">
         <v>154</v>
       </c>
       <c r="I78" t="str">
@@ -3494,26 +4118,26 @@
         <v xml:space="preserve">Please indicate whether you strongly agree, agree, disagree, or strongly disagree with the following statements about the functioning of the civil justice system in [COUNTRY]:Judges in [COUNTRY] decide cases in an independent manner and are not subject to any sort of pressure. </v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="26">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="18">
         <v>8.4</v>
       </c>
-      <c r="B79" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D79" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E79" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G79" s="27" t="s">
+      <c r="B79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="18" t="s">
         <v>13</v>
       </c>
       <c r="I79" t="str">
@@ -3521,8 +4145,8 @@
         <v>NANA</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="33">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="23">
         <v>8.5</v>
       </c>
       <c r="B80" s="8" t="s">
@@ -3537,10 +4161,10 @@
       <c r="E80" t="s">
         <v>28</v>
       </c>
-      <c r="F80" s="9">
+      <c r="F80">
         <v>2019</v>
       </c>
-      <c r="G80" s="9" t="s">
+      <c r="G80" t="s">
         <v>55</v>
       </c>
       <c r="I80" t="str">
@@ -3548,8 +4172,8 @@
         <v>Please tell us how confident you are that the criminal justice system as a whole:Respects the rights of victims.</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="33">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="23">
         <v>8.6</v>
       </c>
       <c r="B81" s="8" t="s">
@@ -3564,10 +4188,10 @@
       <c r="E81" t="s">
         <v>89</v>
       </c>
-      <c r="F81" s="9">
+      <c r="F81">
         <v>2023</v>
       </c>
-      <c r="G81" s="9" t="s">
+      <c r="G81" t="s">
         <v>55</v>
       </c>
       <c r="I81" t="str">
@@ -3575,8 +4199,8 @@
         <v>Please tell us how confident you are that the criminal justice system as a whole:Allows all those accused of crimes to get a fair trial regardless of who they are.</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="33">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="23">
         <v>8.6999999999999993</v>
       </c>
       <c r="B82" s="8" t="s">
@@ -3591,10 +4215,10 @@
       <c r="E82" t="s">
         <v>40</v>
       </c>
-      <c r="F82" s="9">
+      <c r="F82">
         <v>2023</v>
       </c>
-      <c r="G82" s="9" t="s">
+      <c r="G82" t="s">
         <v>159</v>
       </c>
       <c r="I82" t="str">
@@ -3602,13 +4226,1104 @@
         <v>Please tell us how confident you are that the criminal justice system as a whole:Guarantee the safety and human rights of people deprived of their liberty.</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B83" s="8"/>
       <c r="C83" s="3"/>
-      <c r="D83"/>
-      <c r="E83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6225905-0EEB-7941-BBF3-8CA9B35D2D71}">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="45.36328125" customWidth="1"/>
+    <col min="7" max="7" width="40.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>268</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" s="33">
+        <v>1</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="F4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>328</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="50" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>328</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="137.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" t="s">
+        <v>227</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="76" x14ac:dyDescent="0.35">
+      <c r="A9" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="38" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="E10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" t="s">
+        <v>239</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="36" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="H11" s="36">
+        <v>1</v>
+      </c>
+      <c r="I11" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="J11" s="36">
+        <v>2</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="L11" s="36">
+        <v>7</v>
+      </c>
+      <c r="M11" s="36" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="36" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="H12" s="36">
+        <v>1</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="J12" s="36">
+        <v>2</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="L12" s="36">
+        <v>7</v>
+      </c>
+      <c r="M12" s="36" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="50.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" t="s">
+        <v>249</v>
+      </c>
+      <c r="F13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G13" t="s">
+        <v>256</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="63" x14ac:dyDescent="0.35">
+      <c r="A14" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="E15" t="s">
+        <v>249</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="G15" t="s">
+        <v>266</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>325</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="50" x14ac:dyDescent="0.35">
+      <c r="A16" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" t="s">
+        <v>249</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="G16" t="s">
+        <v>273</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="38.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17" t="s">
+        <v>326</v>
+      </c>
+      <c r="J17">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="100" x14ac:dyDescent="0.35">
+      <c r="A18" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="E18" t="s">
+        <v>281</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="E19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F19" t="s">
+        <v>292</v>
+      </c>
+      <c r="G19" t="s">
+        <v>293</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="36" customFormat="1" ht="50" x14ac:dyDescent="0.35">
+      <c r="A20" s="35" t="s">
+        <v>296</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="H20" s="36">
+        <v>4.03</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="36" customFormat="1" ht="50" x14ac:dyDescent="0.35">
+      <c r="A21" s="35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="H21" s="36">
+        <v>4.03</v>
+      </c>
+      <c r="I21" s="36" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="50" x14ac:dyDescent="0.35">
+      <c r="A22" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="E22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="H22" s="32">
+        <v>1</v>
+      </c>
+      <c r="I22" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="J22" s="32">
+        <v>2</v>
+      </c>
+      <c r="K22" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="L22" s="32">
+        <v>7</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E23" t="s">
+        <v>189</v>
+      </c>
+      <c r="F23" t="s">
+        <v>314</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24" t="s">
+        <v>332</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
+    <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <xsd:import namespace="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns2:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="69276225-f05c-44c5-92dc-c999460a4149" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{32d65da7-472f-44c6-be22-218d2da46f49}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="69276225-f05c-44c5-92dc-c999460a4149">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="46f3a809-46a3-44ee-a0f1-42a271529c86" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="10" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c40d4899-0986-466d-9443-4d7b8518a0f2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="21" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="23" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{282C4754-19D9-43CC-B8BD-E8302CC471D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98E61E18-E085-4F32-8BB5-C7E09B0B62F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{775651E1-FBC8-4150-B873-7BBAF7F7B2B5}"/>
 </file>
</xml_diff>